<commit_message>
finish. comments will be added later
</commit_message>
<xml_diff>
--- a/data/Results.xlsx
+++ b/data/Results.xlsx
@@ -1,18 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgorbatenko/Desktop/Pricing model/ICEF_Project/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14180"/>
   </bookViews>
   <sheets>
-    <sheet name="Results" r:id="rId3" sheetId="1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -135,16 +150,27 @@
   </si>
   <si>
     <t>not reject H0 at 5% s.l.</t>
+  </si>
+  <si>
+    <t>Total Z-test</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Significance level</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -156,7 +182,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -171,21 +197,299 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -262,44 +566,44 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="1">
         <v>-2.273123184861825</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="1">
         <v>-1.6145659583527003</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="1">
         <v>-1.680339517246455</v>
       </c>
-      <c r="E2" t="n">
-        <v>-1.149388387981578</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="E2" s="1">
+        <v>-1.1493883879815781</v>
+      </c>
+      <c r="F2" s="1">
         <v>-0.42784463235815884</v>
       </c>
-      <c r="G2" t="n">
-        <v>-0.3683906654825356</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.01150937881485773</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.05320236117761993</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.04644563827404236</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="G2" s="1">
+        <v>-0.36839066548253557</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1.1509378814857731E-2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>5.3202361177619929E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>4.6445638274042363E-2</v>
+      </c>
+      <c r="K2" s="1">
         <v>0.12519793303145454</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2" s="1">
         <v>0.33438211990481315</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>0.35629097834932383</v>
       </c>
       <c r="N2" t="s">
@@ -339,45 +643,45 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.5380042738156116</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-0.2632883830478329</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.6948568622538174</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.264699123800329</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="B3" s="1">
+        <v>0.53800427381561156</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-0.26328838304783292</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.69485686225381738</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.26469912380032901</v>
+      </c>
+      <c r="F3" s="1">
         <v>-0.19891773676012398</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="1">
         <v>-0.18043626463459747</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="1">
         <v>0.29528704901963565</v>
       </c>
-      <c r="I3" t="n">
-        <v>0.3961641564494193</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="I3" s="1">
+        <v>0.39616415644941932</v>
+      </c>
+      <c r="J3" s="1">
         <v>0.2435725044820157</v>
       </c>
-      <c r="K3" t="n">
-        <v>0.3956206262658705</v>
-      </c>
-      <c r="L3" t="n">
+      <c r="K3" s="1">
+        <v>0.39562062626587052</v>
+      </c>
+      <c r="L3" s="1">
         <v>0.42116354741706796</v>
       </c>
-      <c r="M3" t="n">
-        <v>0.4284050432241382</v>
+      <c r="M3">
+        <v>0.42840504322413819</v>
       </c>
       <c r="N3" t="s">
         <v>37</v>
@@ -416,44 +720,44 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="1">
         <v>-0.34403870194498937</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="1">
         <v>-0.26496991059381264</v>
       </c>
-      <c r="D4" t="n">
-        <v>-0.6053734664805183</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4" s="1">
+        <v>-0.60537346648051826</v>
+      </c>
+      <c r="E4" s="1">
         <v>-0.6703233672699056</v>
       </c>
-      <c r="F4" t="n">
-        <v>-0.5780522229592909</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-0.04973946581122487</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.3654085903440794</v>
-      </c>
-      <c r="I4" t="n">
+      <c r="F4" s="1">
+        <v>-0.57805222295929093</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-4.9739465811224869E-2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.36540859034407941</v>
+      </c>
+      <c r="I4" s="1">
         <v>0.39551632071565673</v>
       </c>
-      <c r="J4" t="n">
-        <v>0.2724654384847505</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.2513258371032929</v>
-      </c>
-      <c r="L4" t="n">
+      <c r="J4" s="1">
+        <v>0.27246543848475052</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.25132583710329293</v>
+      </c>
+      <c r="L4" s="1">
         <v>0.28161443094535527</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4">
         <v>0.48016500309852717</v>
       </c>
       <c r="N4" t="s">
@@ -493,45 +797,45 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="n">
-        <v>-1.373182838359917</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5" s="1">
+        <v>-1.3731828383599169</v>
+      </c>
+      <c r="C5" s="1">
         <v>-1.7937379684165229</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="1">
         <v>-1.1855481114755195</v>
       </c>
-      <c r="E5" t="n">
-        <v>-0.7682604287241898</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-0.4845747614165364</v>
-      </c>
-      <c r="G5" t="n">
+      <c r="E5" s="1">
+        <v>-0.76826042872418976</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-0.48457476141653638</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.27173171678388813</v>
       </c>
-      <c r="H5" t="n">
-        <v>0.08484775673719244</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.03642750102560204</v>
-      </c>
-      <c r="J5" t="n">
+      <c r="H5" s="1">
+        <v>8.4847756737192442E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.6427501025602042E-2</v>
+      </c>
+      <c r="J5" s="1">
         <v>0.11790040203932885</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5" s="1">
         <v>0.2211662395010614</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5" s="1">
         <v>0.31398901015806047</v>
       </c>
-      <c r="M5" t="n">
-        <v>0.3929141560521008</v>
+      <c r="M5">
+        <v>0.39291415605210078</v>
       </c>
       <c r="N5" t="s">
         <v>37</v>
@@ -570,44 +874,44 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="n">
-        <v>-0.8373968875581436</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6" s="1">
+        <v>-0.83739688755814357</v>
+      </c>
+      <c r="C6" s="1">
         <v>-1.8224655395049132</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="1">
         <v>-1.5104665313529284</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="1">
         <v>-1.1491259642299116</v>
       </c>
-      <c r="F6" t="n">
-        <v>-0.9677605960594957</v>
-      </c>
-      <c r="G6" t="n">
+      <c r="F6" s="1">
+        <v>-0.96776059605949571</v>
+      </c>
+      <c r="G6" s="1">
         <v>-0.9283850636441362</v>
       </c>
-      <c r="H6" t="n">
-        <v>0.2011847573377191</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.03419218896505077</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.0654622116049201</v>
-      </c>
-      <c r="K6" t="n">
+      <c r="H6" s="1">
+        <v>0.20118475733771909</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3.4192188965050767E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>6.5462211604920106E-2</v>
+      </c>
+      <c r="K6" s="1">
         <v>0.125252021770275</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6" s="1">
         <v>0.16658197360421964</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6">
         <v>0.17660393177925918</v>
       </c>
       <c r="N6" t="s">
@@ -647,44 +951,44 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="n">
-        <v>-0.9091452582793466</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7" s="1">
+        <v>-0.90914525827934656</v>
+      </c>
+      <c r="C7" s="1">
         <v>-3.1801605597357643</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="1">
         <v>-1.6920728908525047</v>
       </c>
-      <c r="E7" t="n">
-        <v>-1.342052211015799</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="E7" s="1">
+        <v>-1.3420522110157991</v>
+      </c>
+      <c r="F7" s="1">
         <v>-1.3382901370527094</v>
       </c>
-      <c r="G7" t="n">
-        <v>-0.7360136231948344</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.1816367277118796</v>
-      </c>
-      <c r="I7" t="n">
-        <v>7.359673593207483E-4</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.04531603827671052</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.08978953369299407</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.09040093785613812</v>
-      </c>
-      <c r="M7" t="n">
+      <c r="G7" s="1">
+        <v>-0.73601362319483443</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.18163672771187961</v>
+      </c>
+      <c r="I7" s="1">
+        <v>7.3596735932074831E-4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>4.5316038276710519E-2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>8.978953369299407E-2</v>
+      </c>
+      <c r="L7" s="1">
+        <v>9.0400937856138119E-2</v>
+      </c>
+      <c r="M7">
         <v>0.23086120356489617</v>
       </c>
       <c r="N7" t="s">
@@ -724,45 +1028,45 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="n">
-        <v>-6.621660101194373</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8" s="1">
+        <v>-6.6216601011943732</v>
+      </c>
+      <c r="C8" s="1">
         <v>-4.444635225566909</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="1">
         <v>-3.7607423036379033</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="1">
         <v>-3.0696877246598646</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="1">
         <v>-2.5908144909794624</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="1">
         <v>-2.8658977784711253</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="1">
         <v>1.7759351891243365E-11</v>
       </c>
-      <c r="I8" t="n">
-        <v>4.402055895315998E-6</v>
-      </c>
-      <c r="J8" t="n">
-        <v>8.470494277405442E-5</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.0010714134598871926</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.004787454512295174</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.002079142469046311</v>
+      <c r="I8" s="1">
+        <v>4.4020558953159979E-6</v>
+      </c>
+      <c r="J8" s="1">
+        <v>8.4704942774054416E-5</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.0714134598871926E-3</v>
+      </c>
+      <c r="L8" s="1">
+        <v>4.7874545122951742E-3</v>
+      </c>
+      <c r="M8">
+        <v>2.0791424690463109E-3</v>
       </c>
       <c r="N8" t="s">
         <v>38</v>
@@ -801,45 +1105,45 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="n">
-        <v>-5.987062271599615</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-3.17162268116019</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="B9" s="1">
+        <v>-5.9870622715996147</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-3.1716226811601902</v>
+      </c>
+      <c r="D9" s="1">
         <v>-2.3879695791065454</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="1">
         <v>-1.790012558807375</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="1">
         <v>-1.7255697939839973</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="1">
         <v>-1.4365236297666024</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9" s="1">
         <v>1.0683249771312718E-9</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" s="1">
         <v>7.579491214963482E-4</v>
       </c>
-      <c r="J9" t="n">
-        <v>0.008470872033626963</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.036725946231766504</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.0422124187299873</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.07542669869564295</v>
+      <c r="J9" s="1">
+        <v>8.4708720336269631E-3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3.6725946231766504E-2</v>
+      </c>
+      <c r="L9" s="1">
+        <v>4.2212418729987301E-2</v>
+      </c>
+      <c r="M9">
+        <v>7.5426698695642946E-2</v>
       </c>
       <c r="N9" t="s">
         <v>38</v>
@@ -878,44 +1182,44 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="1">
         <v>-0.23596572278021935</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="1">
         <v>0.17974563671369514</v>
       </c>
-      <c r="D10" t="n">
-        <v>-0.7306501105329551</v>
-      </c>
-      <c r="E10" t="n">
-        <v>-0.7482559666570842</v>
-      </c>
-      <c r="F10" t="n">
-        <v>-0.7197606111852531</v>
-      </c>
-      <c r="G10" t="n">
-        <v>-0.5882996198420276</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.4067296342156589</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.428676131981817</v>
-      </c>
-      <c r="J10" t="n">
+      <c r="D10" s="1">
+        <v>-0.73065011053295514</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-0.74825596665708416</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-0.71976061118525314</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-0.58829961984202761</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.40672963421565889</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.42867613198181698</v>
+      </c>
+      <c r="J10" s="1">
         <v>0.23249644785660822</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10" s="1">
         <v>0.22715288946591405</v>
       </c>
-      <c r="L10" t="n">
+      <c r="L10" s="1">
         <v>0.23583620027840638</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M10">
         <v>0.27816560036116833</v>
       </c>
       <c r="N10" t="s">
@@ -955,45 +1259,45 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="1">
         <v>6.752503367482551</v>
       </c>
-      <c r="C11" t="n">
-        <v>4.834883375570459</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="C11" s="1">
+        <v>4.8348833755704588</v>
+      </c>
+      <c r="D11" s="1">
         <v>3.1785820180718902</v>
       </c>
-      <c r="E11" t="n">
-        <v>2.18864428279528</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1.307568244262799</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.3185017088403155</v>
-      </c>
-      <c r="H11" t="n">
+      <c r="E11" s="1">
+        <v>2.1886442827952801</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.3075682442627989</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.31850170884031548</v>
+      </c>
+      <c r="H11" s="1">
         <v>7.2657844559589444E-12</v>
       </c>
-      <c r="I11" t="n">
-        <v>6.661185871133355E-7</v>
-      </c>
-      <c r="J11" t="n">
-        <v>7.399867013638609E-4</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.014311352287180024</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.0955098968476182</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.3750521993127415</v>
+      <c r="I11" s="1">
+        <v>6.6611858711333549E-7</v>
+      </c>
+      <c r="J11" s="1">
+        <v>7.3998670136386085E-4</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1.4311352287180024E-2</v>
+      </c>
+      <c r="L11" s="1">
+        <v>9.5509896847618195E-2</v>
+      </c>
+      <c r="M11">
+        <v>0.37505219931274147</v>
       </c>
       <c r="N11" t="s">
         <v>38</v>
@@ -1032,45 +1336,45 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" s="1">
         <v>3.742040768556306</v>
       </c>
-      <c r="C12" t="n">
-        <v>1.113327672839246</v>
-      </c>
-      <c r="D12" t="n">
+      <c r="C12" s="1">
+        <v>1.1133276728392461</v>
+      </c>
+      <c r="D12" s="1">
         <v>1.5518064551170456</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" s="1">
         <v>1.6949874438328134</v>
       </c>
-      <c r="F12" t="n">
-        <v>2.815996452221347</v>
-      </c>
-      <c r="G12" t="n">
+      <c r="F12" s="1">
+        <v>2.8159964522213472</v>
+      </c>
+      <c r="G12" s="1">
         <v>3.2798856941363583</v>
       </c>
-      <c r="H12" t="n">
-        <v>9.126594668439945E-5</v>
-      </c>
-      <c r="I12" t="n">
+      <c r="H12" s="1">
+        <v>9.1265946684399452E-5</v>
+      </c>
+      <c r="I12" s="1">
         <v>0.13278386281052906</v>
       </c>
-      <c r="J12" t="n">
-        <v>0.06035427047105441</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.04503890136515362</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.0024313101825809836</v>
-      </c>
-      <c r="M12" t="n">
-        <v>5.19245764122988E-4</v>
+      <c r="J12" s="1">
+        <v>6.0354270471054412E-2</v>
+      </c>
+      <c r="K12" s="1">
+        <v>4.5038901365153622E-2</v>
+      </c>
+      <c r="L12" s="1">
+        <v>2.4313101825809836E-3</v>
+      </c>
+      <c r="M12">
+        <v>5.1924576412298797E-4</v>
       </c>
       <c r="N12" t="s">
         <v>38</v>
@@ -1109,45 +1413,45 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="1">
         <v>-1.3068595541976054</v>
       </c>
-      <c r="C13" t="n">
-        <v>-0.9207241074122686</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-0.4498610466644012</v>
-      </c>
-      <c r="E13" t="n">
-        <v>-0.597094336291949</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-0.8338098294534966</v>
-      </c>
-      <c r="G13" t="n">
-        <v>-0.666523958509811</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.09563020732101225</v>
-      </c>
-      <c r="I13" t="n">
+      <c r="C13" s="1">
+        <v>-0.92072410741226862</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-0.44986104666440119</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-0.59709433629194897</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-0.83380982945349658</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-0.66652395850981105</v>
+      </c>
+      <c r="H13" s="1">
+        <v>9.5630207321012253E-2</v>
+      </c>
+      <c r="I13" s="1">
         <v>0.1785972432897453</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J13" s="1">
         <v>0.32640531827803854</v>
       </c>
-      <c r="K13" t="n">
+      <c r="K13" s="1">
         <v>0.2752221995245473</v>
       </c>
-      <c r="L13" t="n">
+      <c r="L13" s="1">
         <v>0.20219407772020212</v>
       </c>
-      <c r="M13" t="n">
-        <v>0.2525381275515016</v>
+      <c r="M13">
+        <v>0.25253812755150162</v>
       </c>
       <c r="N13" t="s">
         <v>37</v>
@@ -1186,7 +1490,102 @@
         <v>40</v>
       </c>
     </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1">
+        <f>SUM(B2:B13)/SQRT(COUNT(B2:B13))</f>
+        <v>-2.5564741150266177</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" ref="C15:G15" si="0">SUM(C2:C13)/SQRT(COUNT(C2:C13))</f>
+        <v>-3.2759471024397877</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.4761912827334513</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.0599482601856258</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.6575235814772848</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.1402930365364736</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1">
+        <f>_xlfn.NORM.S.DIST(B15, 1)</f>
+        <v>5.2869468908196826E-3</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:G16" si="1">_xlfn.NORM.S.DIST(C15, 1)</f>
+        <v>5.2654141433528478E-4</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>6.6396205876099864E-3</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9701743682310695E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8706832654057876E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.12708211896508165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="str">
+        <f>IF($B$17&gt;B16, "reject H0 at "&amp;B17&amp;" s.l.","not reject H0 at "&amp;B17&amp;" s.l.")</f>
+        <v>reject H0 at 0.01 s.l.</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" ref="C18:G18" si="2">IF($B$17&gt;C16, "reject H0 at "&amp;C17&amp;" s.l.","not reject H0 at "&amp;C17&amp;" s.l.")</f>
+        <v>reject H0 at  s.l.</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>reject H0 at  s.l.</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>not reject H0 at  s.l.</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>not reject H0 at  s.l.</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>not reject H0 at  s.l.</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>